<commit_message>
mise à jour des fichier act_report.html, requirements.txt
</commit_message>
<xml_diff>
--- a/df_etape_chien.xlsx
+++ b/df_etape_chien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Formation\Udacity\Nanodegree\Analyse_donnees\Projet\projet_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D1F1BF-EAC5-481A-BD4D-C5ABAA0DC26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C40E95-7C05-4187-A32C-30418DE9EB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t>tweet_id</t>
   </si>
@@ -64,15 +64,6 @@
     <t>puppo</t>
   </si>
   <si>
-    <t>user_followers</t>
-  </si>
-  <si>
-    <t>retweet</t>
-  </si>
-  <si>
-    <t>favorite</t>
-  </si>
-  <si>
     <t>&lt;a href="http://twitter.com/download/iphone" rel="nofollow"&gt;Twitter for iPhone&lt;/a&gt;</t>
   </si>
   <si>
@@ -157,13 +148,13 @@
     <t>https://twitter.com/dog_rates/status/854010172552949760/photo/1,https://twitter.com/dog_rates/status/854010172552949760/photo/1</t>
   </si>
   <si>
+    <t>Burke</t>
+  </si>
+  <si>
+    <t>Dexter</t>
+  </si>
+  <si>
     <t>Lila</t>
-  </si>
-  <si>
-    <t>Dexter</t>
-  </si>
-  <si>
-    <t>Burke</t>
   </si>
 </sst>
 </file>
@@ -173,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,14 +176,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,9 +210,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -237,10 +219,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,27 +524,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="107.109375" customWidth="1"/>
-    <col min="8" max="9" width="5.21875" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
-    <col min="16" max="16" width="30.44140625" customWidth="1"/>
+    <col min="7" max="7" width="81.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,116 +578,73 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>460</v>
+      </c>
+      <c r="B3">
+        <v>8.1777768676452352E+17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>42742.707962962973</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>460</v>
-      </c>
-      <c r="B2">
-        <v>8.1777768676452352E+17</v>
-      </c>
-      <c r="E2" s="2">
-        <v>42742.707962962973</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2">
-        <v>114031</v>
-      </c>
-      <c r="Q2">
-        <v>3084</v>
-      </c>
-      <c r="R2">
-        <v>11901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>531</v>
-      </c>
-      <c r="B3">
-        <v>8.0810646058876518E+17</v>
-      </c>
-      <c r="E3" s="2">
-        <v>42716.020462962973</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>114031</v>
-      </c>
-      <c r="Q3">
-        <v>2525</v>
-      </c>
-      <c r="R3">
-        <v>9701</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>531</v>
       </c>
       <c r="B4">
-        <v>8.0810646058876506E+17</v>
+        <v>8.0810646058876518E+17</v>
       </c>
       <c r="E4" s="2">
         <v>42716.020462962973</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -722,66 +653,45 @@
         <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
         <v>12</v>
       </c>
-      <c r="P4">
-        <v>114031</v>
-      </c>
-      <c r="Q4">
-        <v>2525</v>
-      </c>
-      <c r="R4">
-        <v>9701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>565</v>
+        <v>531</v>
       </c>
       <c r="B5">
-        <v>8.0226504815661056E+17</v>
-      </c>
-      <c r="C5">
-        <v>7.3310948527586099E+17</v>
-      </c>
-      <c r="D5">
-        <v>4196983835</v>
+        <v>8.0810646058876518E+17</v>
       </c>
       <c r="E5" s="2">
-        <v>42699.901238425933</v>
+        <v>42716.020462962973</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5">
         <v>10</v>
       </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
       <c r="L5" t="s">
         <v>10</v>
       </c>
-      <c r="P5">
-        <v>114031</v>
-      </c>
-      <c r="Q5">
-        <v>1573</v>
-      </c>
-      <c r="R5">
-        <v>7039</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>565</v>
       </c>
@@ -798,13 +708,13 @@
         <v>42699.901238425933</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>11</v>
@@ -812,146 +722,110 @@
       <c r="J6">
         <v>10</v>
       </c>
-      <c r="N6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P6">
-        <v>114031</v>
-      </c>
-      <c r="Q6">
-        <v>1573</v>
-      </c>
-      <c r="R6">
-        <v>7039</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
+        <v>565</v>
+      </c>
+      <c r="B7">
+        <v>8.0226504815661056E+17</v>
+      </c>
+      <c r="C7">
+        <v>7.3310948527586099E+17</v>
+      </c>
+      <c r="D7">
+        <v>4196983835</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42699.901238425933</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>575</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>8.0111512785250304E+17</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>42696.728067129632</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>705</v>
+      </c>
+      <c r="B9">
+        <v>7.8563975318621798E+17</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42654.02416666667</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="I7">
-        <v>12</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="N7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P7">
-        <v>114031</v>
-      </c>
-      <c r="Q7">
-        <v>2429</v>
-      </c>
-      <c r="R7">
-        <v>8992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>705</v>
-      </c>
-      <c r="B8">
-        <v>7.8563975318621798E+17</v>
-      </c>
-      <c r="E8" s="2">
-        <v>42654.02416666667</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" t="s">
-        <v>12</v>
-      </c>
-      <c r="P8">
-        <v>114031</v>
-      </c>
-      <c r="Q8">
-        <v>2561</v>
-      </c>
-      <c r="R8">
-        <v>8735</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>889</v>
-      </c>
-      <c r="B9">
-        <v>7.5979342226174362E+17</v>
-      </c>
-      <c r="E9" s="2">
-        <v>42582.701874999999</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>10</v>
-      </c>
-      <c r="K9" t="s">
-        <v>33</v>
-      </c>
       <c r="L9" t="s">
         <v>10</v>
       </c>
-      <c r="P9">
-        <v>114031</v>
-      </c>
-      <c r="Q9">
-        <v>2173</v>
-      </c>
-      <c r="R9">
-        <v>6620</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>889</v>
       </c>
@@ -962,116 +836,89 @@
         <v>42582.701874999999</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>889</v>
+      </c>
+      <c r="B11">
+        <v>7.5979342226174362E+17</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42582.701874999999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>956</v>
+      </c>
+      <c r="B12">
+        <v>7.5158384726817997E+17</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42560.047766203701</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H12" t="s">
         <v>32</v>
       </c>
-      <c r="I10">
-        <v>12</v>
-      </c>
-      <c r="J10">
-        <v>10</v>
-      </c>
-      <c r="K10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" t="s">
-        <v>12</v>
-      </c>
-      <c r="P10">
-        <v>114031</v>
-      </c>
-      <c r="Q10">
-        <v>2173</v>
-      </c>
-      <c r="R10">
-        <v>6620</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>956</v>
-      </c>
-      <c r="B11">
-        <v>7.5158384726817997E+17</v>
-      </c>
-      <c r="E11" s="2">
-        <v>42560.047766203701</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11">
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="J11">
-        <v>10</v>
-      </c>
-      <c r="L11" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11">
-        <v>114031</v>
-      </c>
-      <c r="Q11">
-        <v>1265</v>
-      </c>
-      <c r="R11">
-        <v>4849</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>1063</v>
-      </c>
-      <c r="B12">
-        <v>7.4106730681879757E+17</v>
-      </c>
-      <c r="E12" s="2">
-        <v>42531.027638888889</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12">
-        <v>12</v>
-      </c>
       <c r="J12">
         <v>10</v>
       </c>
-      <c r="K12" t="s">
-        <v>38</v>
-      </c>
       <c r="L12" t="s">
         <v>10</v>
       </c>
-      <c r="P12">
-        <v>114031</v>
-      </c>
-      <c r="Q12">
-        <v>3520</v>
-      </c>
-      <c r="R12">
-        <v>10342</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1063</v>
       </c>
@@ -1082,13 +929,13 @@
         <v>42531.027638888889</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I13">
         <v>12</v>
@@ -1097,39 +944,30 @@
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13">
-        <v>114031</v>
-      </c>
-      <c r="Q13">
-        <v>3520</v>
-      </c>
-      <c r="R13">
-        <v>10342</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>1113</v>
+        <v>1063</v>
       </c>
       <c r="B14">
-        <v>7.3310948527586099E+17</v>
+        <v>7.4106730681879757E+17</v>
       </c>
       <c r="E14" s="2">
-        <v>42509.068240740737</v>
+        <v>42531.027638888889</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I14">
         <v>12</v>
@@ -1137,20 +975,14 @@
       <c r="J14">
         <v>10</v>
       </c>
-      <c r="L14" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14">
-        <v>114031</v>
-      </c>
-      <c r="Q14">
-        <v>17621</v>
-      </c>
-      <c r="R14">
-        <v>44619</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1113</v>
       </c>
@@ -1161,113 +993,112 @@
         <v>42509.068240740737</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1113</v>
+      </c>
+      <c r="B16">
+        <v>7.3310948527586099E+17</v>
+      </c>
+      <c r="E16" s="2">
+        <v>42509.068240740737</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>191</v>
+      </c>
+      <c r="B17">
+        <v>8.5585145381401395E+17</v>
+      </c>
+      <c r="E17" s="2">
+        <v>42847.771550925929</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
         <v>39</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I17">
+        <v>13</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="O17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>200</v>
+      </c>
+      <c r="B18">
+        <v>8.5401017255294976E+17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>42842.690578703703</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
         <v>40</v>
       </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>10</v>
-      </c>
-      <c r="N15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P15">
-        <v>114031</v>
-      </c>
-      <c r="Q15">
-        <v>17621</v>
-      </c>
-      <c r="R15">
-        <v>44619</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>191</v>
-      </c>
-      <c r="B16">
-        <v>8.5585145381401395E+17</v>
-      </c>
-      <c r="E16" s="2">
-        <v>42847.771550925929</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H18" t="s">
         <v>41</v>
       </c>
-      <c r="H16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16">
-        <v>13</v>
-      </c>
-      <c r="J16">
-        <v>10</v>
-      </c>
-      <c r="O16" t="s">
-        <v>13</v>
-      </c>
-      <c r="P16">
-        <v>114031</v>
-      </c>
-      <c r="Q16">
-        <v>19196</v>
-      </c>
-      <c r="R16">
-        <v>47844</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>200</v>
-      </c>
-      <c r="B17">
-        <v>8.5401017255294976E+17</v>
-      </c>
-      <c r="E17" s="2">
-        <v>42842.690578703703</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17">
+      <c r="I18">
         <v>11</v>
       </c>
-      <c r="J17">
-        <v>10</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="M18" t="s">
         <v>11</v>
       </c>
-      <c r="P17">
-        <v>114031</v>
-      </c>
-      <c r="Q17">
-        <v>3433</v>
-      </c>
-      <c r="R17">
-        <v>17169</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1" xr:uid="{E172A0DD-528D-4DBD-8DEE-367930B0CBBC}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>